<commit_message>
1.1 use template excel to output
</commit_message>
<xml_diff>
--- a/模板.xlsx
+++ b/模板.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sssimonyang\projects\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4732A96-71FD-4F9B-86C7-A4001CACA037}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672D4373-76E8-47EB-9255-EBF7936B0537}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>9点35分前有上千白单，且9点32分至14点55分无上千买单或者上千卖单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>9点35分前有连续白单（均大于100，小于1000）（中间夹单不超过五个），且全天无901以上的买单或卖单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1.按现手大小排序</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -58,6 +50,14 @@
   </si>
   <si>
     <t>9点32分前有白单（大于100，小于1000），且全天无901以上买单或卖单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9点35分前有上千白单，且全天无1001以上买单或卖单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9点35分前有连续白单（均大于100，小于1000）（中间夹单不超过五个），且全天无901以上买单或卖单</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -457,7 +457,7 @@
   <dimension ref="A1:G385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -468,19 +468,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -501,7 +501,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -512,7 +512,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2"/>
     </row>

</xml_diff>

<commit_message>
1.2 change some condition
</commit_message>
<xml_diff>
--- a/模板.xlsx
+++ b/模板.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sssimonyang\projects\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672D4373-76E8-47EB-9255-EBF7936B0537}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F61B27-FA09-43EE-B6C1-7A36D8740DFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -27,11 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>9点35分前有连续上千白单（中间夹单不超过五个）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>1.按现手大小排序</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -42,10 +38,6 @@
   </si>
   <si>
     <t>3.全天是从9点32分至14点57分，不含尾盘</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>9点35分前有上万白单</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -60,12 +52,24 @@
     <t>9点35分前有连续白单（均大于100，小于1000）（中间夹单不超过五个），且全天无901以上买单或卖单</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>9点35分前有上万白单，且全天无10001以上买单或卖单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9点35分前有连续上千白单（中间夹单不超过五个），且全天无9001以上买单或卖单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.9点35分前是从9点30分至9点35分</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="宋体"/>
@@ -88,12 +92,6 @@
       <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -126,7 +124,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -145,11 +143,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -457,30 +452,30 @@
   <dimension ref="A1:G385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="21.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="48" style="7" customWidth="1"/>
+    <col min="1" max="5" width="21.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="48" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -490,7 +485,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -501,7 +496,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -511,8 +506,8 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="8" t="s">
-        <v>3</v>
+      <c r="F4" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -522,7 +517,9 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>